<commit_message>
Fixed EROR Title is more than 31 characters
</commit_message>
<xml_diff>
--- a/Horario_Semana_Completo.xlsx
+++ b/Horario_Semana_Completo.xlsx
@@ -7,38 +7,38 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="lunes-Asistente de Self Checkout" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="lunes-Representante de Servicio" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="lunes-Self Checkout" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="lunes-RS" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="lunes-Cajer@" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="lunes-Ecommerce" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="lunes-Supervisor(@)" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="martes-Asistente de Self Checkout" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="martes-Representante de Servicio" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="martes-Self Checkout" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="martes-RS" sheetId="7" state="visible" r:id="rId7"/>
     <sheet name="martes-Cajer@" sheetId="8" state="visible" r:id="rId8"/>
     <sheet name="martes-Ecommerce" sheetId="9" state="visible" r:id="rId9"/>
     <sheet name="martes-Supervisor(@)" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="miércoles-Asistente de Self Checkout" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet name="miércoles-Representante de Servicio" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="miércoles-Self Checkout" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="miércoles-RS" sheetId="12" state="visible" r:id="rId12"/>
     <sheet name="miércoles-Cajer@" sheetId="13" state="visible" r:id="rId13"/>
     <sheet name="miércoles-Ecommerce" sheetId="14" state="visible" r:id="rId14"/>
     <sheet name="miércoles-Supervisor(@)" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet name="jueves-Asistente de Self Checkout" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet name="jueves-Representante de Servicio" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="jueves-Self Checkout" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="jueves-RS" sheetId="17" state="visible" r:id="rId17"/>
     <sheet name="jueves-Cajer@" sheetId="18" state="visible" r:id="rId18"/>
     <sheet name="jueves-Ecommerce" sheetId="19" state="visible" r:id="rId19"/>
     <sheet name="jueves-Supervisor(@)" sheetId="20" state="visible" r:id="rId20"/>
-    <sheet name="viernes-Asistente de Self Checkout" sheetId="21" state="visible" r:id="rId21"/>
-    <sheet name="viernes-Representante de Servicio" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet name="viernes-Self Checkout" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet name="viernes-RS" sheetId="22" state="visible" r:id="rId22"/>
     <sheet name="viernes-Cajer@" sheetId="23" state="visible" r:id="rId23"/>
     <sheet name="viernes-Ecommerce" sheetId="24" state="visible" r:id="rId24"/>
     <sheet name="viernes-Supervisor(@)" sheetId="25" state="visible" r:id="rId25"/>
-    <sheet name="sábado-Asistente de Self Checkout" sheetId="26" state="visible" r:id="rId26"/>
-    <sheet name="sábado-Representante de Servicio" sheetId="27" state="visible" r:id="rId27"/>
+    <sheet name="sábado-Self Checkout" sheetId="26" state="visible" r:id="rId26"/>
+    <sheet name="sábado-RS" sheetId="27" state="visible" r:id="rId27"/>
     <sheet name="sábado-Cajer@" sheetId="28" state="visible" r:id="rId28"/>
     <sheet name="sábado-Ecommerce" sheetId="29" state="visible" r:id="rId29"/>
     <sheet name="sábado-Supervisor(@)" sheetId="30" state="visible" r:id="rId30"/>
-    <sheet name="domingo-Asistente de Self Checkout" sheetId="31" state="visible" r:id="rId31"/>
-    <sheet name="domingo-Representante de Servicio" sheetId="32" state="visible" r:id="rId32"/>
+    <sheet name="domingo-Self Checkout" sheetId="31" state="visible" r:id="rId31"/>
+    <sheet name="domingo-RS" sheetId="32" state="visible" r:id="rId32"/>
     <sheet name="domingo-Cajer@" sheetId="33" state="visible" r:id="rId33"/>
     <sheet name="domingo-Ecommerce" sheetId="34" state="visible" r:id="rId34"/>
     <sheet name="domingo-Supervisor(@)" sheetId="35" state="visible" r:id="rId35"/>

</xml_diff>